<commit_message>
Cleaned and added Delebrate invocation of Exception and Handling
</commit_message>
<xml_diff>
--- a/src/main/resources/input/RetailRewardLog.xlsx
+++ b/src/main/resources/input/RetailRewardLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katta\eclipse-workspace\rewardapp\src\main\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891543B2-D26D-41AC-B2D7-10FE86826210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB547F8-67E9-410B-ACB8-38BBE032DB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A9281018-2E16-4E43-97F5-81EEAB884631}"/>
+    <workbookView xWindow="1720" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{A9281018-2E16-4E43-97F5-81EEAB884631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Customer ID</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Gate</t>
+  </si>
+  <si>
+    <t>3 Month Summary</t>
   </si>
 </sst>
 </file>
@@ -95,15 +98,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -111,17 +126,166 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,156 +600,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA3BB0C-FB44-4991-AD9E-C369F9BAC4EA}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="3"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="22" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="F1" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>44851</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="7">
         <v>49</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="5">
         <v>44858</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
         <v>70</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="5">
         <v>44875</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>90</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="B5" s="5">
         <v>44915</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="7">
         <v>220</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>290</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="F5" s="8">
+        <f>E2+E3+E4+E5</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="B6" s="5">
         <v>44844</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="7">
         <v>120</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>2</v>
       </c>
       <c r="B7" s="5">
         <v>44875</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="7">
         <v>30</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>2</v>
       </c>
       <c r="B8" s="5">
         <v>44905</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="7">
         <v>100</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>50</v>
       </c>
-    </row>
+      <c r="F8" s="8">
+        <f>E6+E7+E8</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Logic and added comments
</commit_message>
<xml_diff>
--- a/src/main/resources/input/RetailRewardLog.xlsx
+++ b/src/main/resources/input/RetailRewardLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katta\eclipse-workspace\rewardapp\src\main\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB547F8-67E9-410B-ACB8-38BBE032DB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5729908-4102-4B0B-B6D6-7E065B36502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{A9281018-2E16-4E43-97F5-81EEAB884631}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="A9" sqref="A9:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>